<commit_message>
Se sube la última versión del código
</commit_message>
<xml_diff>
--- a/docs/asignaturas.xlsx
+++ b/docs/asignaturas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j-ase\Documents\TFG\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD2869-178C-4081-8445-E9B79514E7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7E3B5-E027-414D-B584-EC55E0C020D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="2700" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="85">
   <si>
     <t>NOMBRE ASIGNATURA</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>ORGANIZACIÓN DE COMPUTADORES</t>
+  </si>
+  <si>
+    <t>CUATRIMESTRE</t>
   </si>
 </sst>
 </file>
@@ -632,10 +635,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,9 +648,10 @@
     <col min="3" max="3" width="11.42578125" style="2"/>
     <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
@@ -672,8 +676,11 @@
       <c r="H1" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42300</v>
       </c>
@@ -686,8 +693,11 @@
       <c r="D2" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42301</v>
       </c>
@@ -700,8 +710,11 @@
       <c r="D3" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42302</v>
       </c>
@@ -714,8 +727,11 @@
       <c r="D4" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42303</v>
       </c>
@@ -728,8 +744,11 @@
       <c r="D5" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42304</v>
       </c>
@@ -742,8 +761,11 @@
       <c r="D6" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42305</v>
       </c>
@@ -756,8 +778,11 @@
       <c r="D7" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42306</v>
       </c>
@@ -770,8 +795,11 @@
       <c r="D8" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42307</v>
       </c>
@@ -784,8 +812,11 @@
       <c r="D9" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42308</v>
       </c>
@@ -798,8 +829,11 @@
       <c r="D10" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42309</v>
       </c>
@@ -812,8 +846,11 @@
       <c r="D11" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42310</v>
       </c>
@@ -826,8 +863,11 @@
       <c r="D12" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42311</v>
       </c>
@@ -840,8 +880,11 @@
       <c r="D13" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42312</v>
       </c>
@@ -854,8 +897,11 @@
       <c r="D14" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42313</v>
       </c>
@@ -868,8 +914,11 @@
       <c r="D15" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42314</v>
       </c>
@@ -882,8 +931,11 @@
       <c r="D16" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42315</v>
       </c>
@@ -896,8 +948,11 @@
       <c r="D17" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42316</v>
       </c>
@@ -910,8 +965,11 @@
       <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42317</v>
       </c>
@@ -924,8 +982,11 @@
       <c r="D19" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42318</v>
       </c>
@@ -938,8 +999,11 @@
       <c r="D20" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42319</v>
       </c>
@@ -952,8 +1016,11 @@
       <c r="D21" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42320</v>
       </c>
@@ -966,8 +1033,11 @@
       <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42321</v>
       </c>
@@ -980,8 +1050,11 @@
       <c r="D23" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42322</v>
       </c>
@@ -994,8 +1067,11 @@
       <c r="D24" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42323</v>
       </c>
@@ -1008,8 +1084,11 @@
       <c r="D25" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42324</v>
       </c>
@@ -1022,8 +1101,11 @@
       <c r="D26" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42325</v>
       </c>
@@ -1036,8 +1118,11 @@
       <c r="D27" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42326</v>
       </c>
@@ -1050,8 +1135,11 @@
       <c r="D28" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42327</v>
       </c>
@@ -1064,8 +1152,11 @@
       <c r="D29" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42328</v>
       </c>
@@ -1078,8 +1169,11 @@
       <c r="D30" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42329</v>
       </c>
@@ -1092,8 +1186,11 @@
       <c r="D31" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42330</v>
       </c>
@@ -1106,8 +1203,11 @@
       <c r="D32" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>42331</v>
       </c>
@@ -1120,8 +1220,11 @@
       <c r="D33" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>42332</v>
       </c>
@@ -1134,8 +1237,11 @@
       <c r="D34" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42333</v>
       </c>
@@ -1148,8 +1254,11 @@
       <c r="D35" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42334</v>
       </c>
@@ -1162,8 +1271,11 @@
       <c r="D36" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>42335</v>
       </c>
@@ -1176,8 +1288,11 @@
       <c r="D37" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>42336</v>
       </c>
@@ -1190,8 +1305,11 @@
       <c r="D38" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>42337</v>
       </c>
@@ -1204,8 +1322,11 @@
       <c r="D39" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42338</v>
       </c>
@@ -1218,8 +1339,11 @@
       <c r="D40" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42339</v>
       </c>
@@ -1232,8 +1356,11 @@
       <c r="D41" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42340</v>
       </c>
@@ -1246,8 +1373,11 @@
       <c r="D42" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42341</v>
       </c>
@@ -1260,8 +1390,11 @@
       <c r="D43" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42342</v>
       </c>
@@ -1274,8 +1407,11 @@
       <c r="D44" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42343</v>
       </c>
@@ -1288,8 +1424,11 @@
       <c r="D45" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42344</v>
       </c>
@@ -1302,8 +1441,11 @@
       <c r="D46" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>42345</v>
       </c>
@@ -1316,8 +1458,11 @@
       <c r="D47" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>42346</v>
       </c>
@@ -1330,8 +1475,11 @@
       <c r="D48" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>42347</v>
       </c>
@@ -1344,8 +1492,11 @@
       <c r="D49" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>42348</v>
       </c>
@@ -1358,8 +1509,11 @@
       <c r="D50" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>42349</v>
       </c>
@@ -1372,8 +1526,11 @@
       <c r="D51" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>42350</v>
       </c>
@@ -1386,8 +1543,11 @@
       <c r="D52" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>42351</v>
       </c>
@@ -1400,8 +1560,11 @@
       <c r="D53" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>42352</v>
       </c>
@@ -1414,8 +1577,11 @@
       <c r="D54" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>42353</v>
       </c>
@@ -1428,8 +1594,11 @@
       <c r="D55" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42354</v>
       </c>
@@ -1442,8 +1611,11 @@
       <c r="D56" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>42355</v>
       </c>
@@ -1456,8 +1628,11 @@
       <c r="D57" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>42356</v>
       </c>
@@ -1470,8 +1645,11 @@
       <c r="D58" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>42357</v>
       </c>
@@ -1484,8 +1662,11 @@
       <c r="D59" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>42358</v>
       </c>
@@ -1498,8 +1679,11 @@
       <c r="D60" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>42361</v>
       </c>
@@ -1512,8 +1696,11 @@
       <c r="D61" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42362</v>
       </c>
@@ -1526,8 +1713,11 @@
       <c r="D62" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42364</v>
       </c>
@@ -1540,8 +1730,11 @@
       <c r="D63" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42366</v>
       </c>
@@ -1554,8 +1747,11 @@
       <c r="D64" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42367</v>
       </c>
@@ -1568,8 +1764,11 @@
       <c r="D65" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42371</v>
       </c>
@@ -1582,8 +1781,11 @@
       <c r="D66" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42377</v>
       </c>
@@ -1596,8 +1798,11 @@
       <c r="D67" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>42378</v>
       </c>
@@ -1610,8 +1815,11 @@
       <c r="D68" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>42379</v>
       </c>
@@ -1624,8 +1832,11 @@
       <c r="D69" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>42380</v>
       </c>
@@ -1638,8 +1849,11 @@
       <c r="D70" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>42399</v>
       </c>
@@ -1651,6 +1865,9 @@
       </c>
       <c r="D71" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="I71">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>